<commit_message>
sua css man signup + navbar
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\study stuffs\swp - group projec t\phan lam cua nhom\tuan 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\study stuffs\swp - group projec t\phan lam cua nhom\SWP391_SE1630-NET_Group1\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238C89B0-EE3A-46BC-B42B-6CE04CB2884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D9E388-833F-447B-B34F-2606072ECA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="65">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Nguyễn Duy Hưng</t>
   </si>
   <si>
-    <t>Lê Hoàng Anh, Vũ Nhật Minh</t>
-  </si>
-  <si>
     <t>Vũ Nhật Minh</t>
   </si>
   <si>
@@ -215,6 +212,18 @@
   </si>
   <si>
     <t>DucDT</t>
+  </si>
+  <si>
+    <t>HungND, DucDT</t>
+  </si>
+  <si>
+    <t>Lê Hoàng Anh (FE-50), Vũ Nhật Minh (BE-50)</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy Hưng (FE-50), Đặng Trần Đức (BE-50)</t>
+  </si>
+  <si>
+    <t>Lê Hoàng Anh (FE)</t>
   </si>
 </sst>
 </file>
@@ -859,8 +868,8 @@
   </sheetPr>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -942,10 +951,10 @@
         <v>6</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>6</v>
@@ -965,10 +974,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>6</v>
@@ -991,7 +1000,7 @@
         <v>59</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>6</v>
@@ -1014,7 +1023,7 @@
         <v>59</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>6</v>
@@ -1034,10 +1043,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>6</v>
@@ -1057,10 +1066,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>6</v>
@@ -1079,11 +1088,11 @@
       <c r="D15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>52</v>
+      <c r="E15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>6</v>
@@ -1103,10 +1112,10 @@
         <v>6</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>6</v>
@@ -1126,10 +1135,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>6</v>
@@ -1149,7 +1158,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>51</v>
@@ -1172,7 +1181,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>52</v>
@@ -1195,7 +1204,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>52</v>
@@ -1218,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>52</v>
@@ -1241,10 +1250,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>48</v>
@@ -1264,10 +1273,10 @@
         <v>8</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>48</v>
@@ -1287,10 +1296,10 @@
         <v>8</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>48</v>
@@ -1310,10 +1319,10 @@
         <v>8</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>48</v>
@@ -1333,10 +1342,10 @@
         <v>8</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>48</v>
@@ -1356,10 +1365,10 @@
         <v>8</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>48</v>
@@ -1379,10 +1388,10 @@
         <v>8</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>48</v>
@@ -1402,10 +1411,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>48</v>
@@ -1425,7 +1434,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>50</v>
@@ -1448,7 +1457,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>50</v>
@@ -1471,7 +1480,7 @@
         <v>10</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>50</v>
@@ -1494,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>50</v>
@@ -1517,7 +1526,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
cap nhat lai backlog
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -5,30 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\study stuffs\swp - group projec t\phan lam cua nhom\SWP391_SE1630-NET_Group1\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Material\SWP391 - ki moi\phan cua nhom\Source Code\SWP391_SE1630-NET_Group1\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D9E388-833F-447B-B34F-2606072ECA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F163577-F64F-46CB-8BF8-A92D2D25FB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$E$1:$E$32</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="69">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -196,34 +204,46 @@
     <t>Nguyễn Anh Tuấn</t>
   </si>
   <si>
-    <t>MinhVN</t>
-  </si>
-  <si>
-    <t>HungND</t>
-  </si>
-  <si>
-    <t>TuanNA</t>
-  </si>
-  <si>
-    <t>AnhLH</t>
-  </si>
-  <si>
-    <t>AnhLH, MinhVH</t>
-  </si>
-  <si>
-    <t>DucDT</t>
-  </si>
-  <si>
-    <t>HungND, DucDT</t>
-  </si>
-  <si>
-    <t>Lê Hoàng Anh (FE-50), Vũ Nhật Minh (BE-50)</t>
-  </si>
-  <si>
-    <t>Nguyễn Duy Hưng (FE-50), Đặng Trần Đức (BE-50)</t>
-  </si>
-  <si>
-    <t>Lê Hoàng Anh (FE)</t>
+    <t>SRS Status</t>
+  </si>
+  <si>
+    <t>Design Status</t>
+  </si>
+  <si>
+    <t>Coding Status</t>
+  </si>
+  <si>
+    <t>Testing Status</t>
+  </si>
+  <si>
+    <t>% Completed</t>
+  </si>
+  <si>
+    <t>Completed in Iteration</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>HE130782</t>
+  </si>
+  <si>
+    <t>HE151491</t>
+  </si>
+  <si>
+    <t>HE130080</t>
+  </si>
+  <si>
+    <t>HE130118</t>
+  </si>
+  <si>
+    <t>HE153050</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -405,7 +425,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -465,6 +485,23 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -497,7 +534,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>8980</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -866,55 +903,63 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
-    <col min="6" max="6" width="79.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="225" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="10.44140625" style="27" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" customWidth="1"/>
+    <col min="7" max="7" width="79.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" customWidth="1"/>
+    <col min="15" max="226" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="28"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:14" ht="19.2" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -924,20 +969,41 @@
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
@@ -947,20 +1013,41 @@
       <c r="C9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="18">
+        <v>300</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="33">
+        <v>30</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
@@ -970,20 +1057,41 @@
       <c r="C10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="23" t="s">
+      <c r="D10" s="18">
+        <v>300</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="33">
+        <v>30</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
@@ -993,20 +1101,41 @@
       <c r="C11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="23" t="s">
+      <c r="D11" s="18">
+        <v>100</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="33">
+        <v>30</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
@@ -1016,20 +1145,41 @@
       <c r="C12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="23" t="s">
+      <c r="D12" s="18">
+        <v>200</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="33">
+        <v>30</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>21</v>
       </c>
@@ -1039,20 +1189,41 @@
       <c r="C13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="18">
+        <v>300</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="33">
+        <v>30</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>23</v>
       </c>
@@ -1062,20 +1233,41 @@
       <c r="C14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="18">
+        <v>300</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="33">
+        <v>30</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>41</v>
       </c>
@@ -1085,20 +1277,41 @@
       <c r="C15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="18">
+        <v>100</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="33">
+        <v>30</v>
+      </c>
+      <c r="N15" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>36</v>
       </c>
@@ -1108,20 +1321,41 @@
       <c r="C16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="D16" s="18">
+        <v>300</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" s="33">
+        <v>30</v>
+      </c>
+      <c r="N16" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>38</v>
       </c>
@@ -1131,20 +1365,41 @@
       <c r="C17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="23" t="s">
+      <c r="D17" s="18">
+        <v>200</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" s="33">
+        <v>30</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>42</v>
       </c>
@@ -1154,20 +1409,39 @@
       <c r="C18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" s="33">
+        <v>10</v>
+      </c>
+      <c r="N18" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>24</v>
       </c>
@@ -1177,20 +1451,39 @@
       <c r="C19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="33">
+        <v>10</v>
+      </c>
+      <c r="N19" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>25</v>
       </c>
@@ -1200,20 +1493,39 @@
       <c r="C20" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="20"/>
+      <c r="E20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20" s="33">
+        <v>10</v>
+      </c>
+      <c r="N20" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>26</v>
       </c>
@@ -1223,20 +1535,39 @@
       <c r="C21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="33">
+        <v>10</v>
+      </c>
+      <c r="N21" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>40</v>
       </c>
@@ -1246,20 +1577,39 @@
       <c r="C22" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M22" s="33">
+        <v>10</v>
+      </c>
+      <c r="N22" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>39</v>
       </c>
@@ -1269,20 +1619,39 @@
       <c r="C23" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="20"/>
+      <c r="E23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" s="33">
+        <v>10</v>
+      </c>
+      <c r="N23" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>17</v>
       </c>
@@ -1292,20 +1661,39 @@
       <c r="C24" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" s="33">
+        <v>10</v>
+      </c>
+      <c r="N24" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>29</v>
       </c>
@@ -1315,20 +1703,39 @@
       <c r="C25" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="20"/>
+      <c r="E25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M25" s="33">
+        <v>10</v>
+      </c>
+      <c r="N25" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>30</v>
       </c>
@@ -1338,20 +1745,39 @@
       <c r="C26" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M26" s="33">
+        <v>10</v>
+      </c>
+      <c r="N26" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -1361,20 +1787,39 @@
       <c r="C27" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M27" s="33">
+        <v>10</v>
+      </c>
+      <c r="N27" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -1384,20 +1829,39 @@
       <c r="C28" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="20"/>
+      <c r="E28" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L28" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M28" s="33">
+        <v>10</v>
+      </c>
+      <c r="N28" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
@@ -1407,20 +1871,39 @@
       <c r="C29" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="20"/>
+      <c r="E29" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K29" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M29" s="33">
+        <v>10</v>
+      </c>
+      <c r="N29" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -1430,20 +1913,39 @@
       <c r="C30" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="20"/>
+      <c r="E30" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K30" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M30" s="33">
+        <v>10</v>
+      </c>
+      <c r="N30" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>31</v>
       </c>
@@ -1453,20 +1955,39 @@
       <c r="C31" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="21"/>
+      <c r="E31" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L31" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M31" s="33">
+        <v>10</v>
+      </c>
+      <c r="N31" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>32</v>
       </c>
@@ -1476,20 +1997,39 @@
       <c r="C32" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="21"/>
+      <c r="E32" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L32" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M32" s="33">
+        <v>10</v>
+      </c>
+      <c r="N32" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>43</v>
       </c>
@@ -1499,20 +2039,39 @@
       <c r="C33" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="21"/>
+      <c r="E33" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L33" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M33" s="33">
+        <v>10</v>
+      </c>
+      <c r="N33" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>44</v>
       </c>
@@ -1522,49 +2081,74 @@
       <c r="C34" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="21"/>
+      <c r="E34" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F36" s="24" t="s">
+      <c r="I34" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M34" s="33">
+        <v>10</v>
+      </c>
+      <c r="N34" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G36" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F37" s="24" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G37" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F38" s="24" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G38" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="D1:D32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D32">
-    <sortCondition ref="D32"/>
+  <autoFilter ref="E1:E32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:E32">
+    <sortCondition ref="E32"/>
   </sortState>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C34" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C34 D18:D34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Simple, Medium, Complex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G17" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H17" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D34" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E34" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9:N17" xr:uid="{0E0AE8B6-4FAE-4784-8F99-CA0728E3B816}">
+      <formula1>"Iteration 1, Iteration 2, Iteration 3, Iteration 4, Final"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:L34" xr:uid="{ADAE5CB3-FF0B-4D87-ADAA-6BBDE5986549}">
+      <formula1>"Doing,Pending,Done,Completed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cap nhat backlog + code
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\study stuffs\swp - group projec t\phan lam cua nhom\SWP391_SE1630-NET_Group1\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Material\SWP391 - ki moi\phan cua nhom\Source Code\SWP391_SE1630-NET_Group1\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD922CC5-6A81-4997-B97F-48E552A8E71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CF7D09-BC42-4658-A48F-F0AAD929604E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="71">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Products List (Customer)</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -933,60 +936,60 @@
   </sheetPr>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="4" width="10.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" customWidth="1"/>
-    <col min="15" max="226" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="4" width="10.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" customWidth="1"/>
+    <col min="15" max="226" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="19.2" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>19</v>
       </c>
@@ -1038,10 +1041,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="18">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>6</v>
@@ -1056,25 +1059,25 @@
         <v>6</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>65</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="M9" s="5">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -1082,10 +1085,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="18">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>6</v>
@@ -1100,25 +1103,25 @@
         <v>6</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>65</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="M10" s="5">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
@@ -1126,10 +1129,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="18">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>6</v>
@@ -1144,7 +1147,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>65</v>
@@ -1156,13 +1159,13 @@
         <v>65</v>
       </c>
       <c r="M11" s="5">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>69</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>6</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>65</v>
@@ -1200,13 +1203,13 @@
         <v>65</v>
       </c>
       <c r="M12" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>18</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>6</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>65</v>
@@ -1250,7 +1253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>34</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>65</v>
@@ -1288,13 +1291,13 @@
         <v>65</v>
       </c>
       <c r="M14" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="18">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>6</v>
@@ -1320,7 +1323,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>65</v>
@@ -1332,13 +1335,13 @@
         <v>65</v>
       </c>
       <c r="M15" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>39</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="18">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>6</v>
@@ -1364,7 +1367,7 @@
         <v>6</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>65</v>
@@ -1382,7 +1385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>17</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>66</v>
@@ -1426,7 +1429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>46</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>66</v>
@@ -1470,7 +1473,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
@@ -1496,7 +1499,7 @@
         <v>46</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>66</v>
@@ -1514,7 +1517,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>27</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>46</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>66</v>
@@ -1558,7 +1561,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>46</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>66</v>
@@ -1602,7 +1605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>38</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>46</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>66</v>
@@ -1646,7 +1649,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>46</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>66</v>
@@ -1690,7 +1693,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>32</v>
       </c>
@@ -1716,7 +1719,7 @@
         <v>46</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>66</v>
@@ -1734,7 +1737,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>33</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>46</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>66</v>
@@ -1778,7 +1781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>28</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>46</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>66</v>
@@ -1822,7 +1825,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>31</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>46</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>66</v>
@@ -1866,7 +1869,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
         <v>22</v>
       </c>
@@ -1892,7 +1895,7 @@
         <v>47</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>66</v>
@@ -1910,7 +1913,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
         <v>23</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>47</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>66</v>
@@ -1954,7 +1957,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
         <v>68</v>
       </c>
@@ -1980,7 +1983,7 @@
         <v>47</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>66</v>
@@ -1998,7 +2001,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>29</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>47</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>66</v>
@@ -2042,7 +2045,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>47</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>66</v>
@@ -2086,7 +2089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>41</v>
       </c>
@@ -2112,7 +2115,7 @@
         <v>47</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>66</v>
@@ -2130,7 +2133,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>42</v>
       </c>
@@ -2156,7 +2159,7 @@
         <v>47</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>66</v>
@@ -2174,22 +2177,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G36" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G37" s="24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G38" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="E1:E32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:E32">

</xml_diff>

<commit_message>
chinh sua comment va cac thu
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Material\SWP391 - ki moi\phan cua nhom\Source Code\SWP391_SE1630-NET_Group1\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\study stuffs\swp - group projec t\phan lam cua nhom\SWP391_SE1630-NET_Group1\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CF7D09-BC42-4658-A48F-F0AAD929604E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300D05AB-D704-4972-9BC3-AC8362B95C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="72">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>|</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -440,6 +443,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -449,7 +463,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -527,6 +541,7 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -934,62 +949,62 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="4" width="10.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="29.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="13" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" customWidth="1"/>
-    <col min="15" max="226" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="4" width="10.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="13" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="226" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:14" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1048,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>19</v>
       </c>
@@ -1077,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -1121,7 +1136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
@@ -1165,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>69</v>
       </c>
@@ -1209,7 +1224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>18</v>
       </c>
@@ -1253,7 +1268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>34</v>
       </c>
@@ -1297,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
@@ -1341,7 +1356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>39</v>
       </c>
@@ -1385,7 +1400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>17</v>
       </c>
@@ -1429,7 +1444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
@@ -1516,8 +1531,11 @@
       <c r="N19" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>27</v>
       </c>
@@ -1561,7 +1579,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
@@ -1604,8 +1622,11 @@
       <c r="N21" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>38</v>
       </c>
@@ -1649,7 +1670,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -1693,7 +1714,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>32</v>
       </c>
@@ -1737,7 +1758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>33</v>
       </c>
@@ -1781,7 +1802,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>28</v>
       </c>
@@ -1824,8 +1845,11 @@
       <c r="N26" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>31</v>
       </c>
@@ -1869,7 +1893,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>22</v>
       </c>
@@ -1913,7 +1937,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>23</v>
       </c>
@@ -1957,7 +1981,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
         <v>68</v>
       </c>
@@ -2001,7 +2025,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>29</v>
       </c>
@@ -2045,7 +2069,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
@@ -2089,7 +2113,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>41</v>
       </c>
@@ -2133,7 +2157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>42</v>
       </c>
@@ -2177,22 +2201,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G36" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G37" s="24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G38" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="E1:E32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:E32">

</xml_diff>